<commit_message>
Monster commint. Neglected commiting for some time
</commit_message>
<xml_diff>
--- a/doc/pwmmeres.xlsx
+++ b/doc/pwmmeres.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Tarsoly\Dokumentumok\BME\6. félév\Önlab\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3809F30C-CE77-48A4-B294-E091B519923C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F395A7C6-B3E9-4892-8F31-08330BBD3014}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{E7EDF6E2-79E5-4ECD-836C-5D395DB23DD8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="1" xr2:uid="{E7EDF6E2-79E5-4ECD-836C-5D395DB23DD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Munka2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -72,6 +73,15 @@
   </si>
   <si>
     <t>1% a min</t>
+  </si>
+  <si>
+    <t>akad</t>
+  </si>
+  <si>
+    <t>lassan, lánctalp néha megakad</t>
+  </si>
+  <si>
+    <t>lassan</t>
   </si>
 </sst>
 </file>
@@ -110,10 +120,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -431,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A163B84-C878-4D5D-9C00-5CB0AD431B42}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,25 +454,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
       <c r="C2">
         <v>50</v>
       </c>
@@ -492,7 +502,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -515,7 +525,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="1"/>
       <c r="B4">
         <v>20</v>
       </c>
@@ -533,7 +543,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="1"/>
       <c r="B5">
         <v>30</v>
       </c>
@@ -545,7 +555,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="1"/>
       <c r="B6">
         <v>40</v>
       </c>
@@ -557,7 +567,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="1"/>
       <c r="B7">
         <v>50</v>
       </c>
@@ -566,7 +576,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="1"/>
       <c r="B8">
         <v>60</v>
       </c>
@@ -575,13 +585,13 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="1"/>
       <c r="B9">
         <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="1"/>
       <c r="B10">
         <v>80</v>
       </c>
@@ -593,7 +603,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="1"/>
       <c r="B11">
         <v>90</v>
       </c>
@@ -602,7 +612,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="1"/>
       <c r="B12">
         <v>100</v>
       </c>
@@ -619,4 +629,143 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AEDB21-F2E2-4EFA-AF5C-7D56F6AD6483}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
+      </c>
+      <c r="F2">
+        <v>500</v>
+      </c>
+      <c r="G2">
+        <v>1000</v>
+      </c>
+      <c r="H2">
+        <v>5000</v>
+      </c>
+      <c r="I2">
+        <v>10000</v>
+      </c>
+      <c r="J2">
+        <v>20000</v>
+      </c>
+      <c r="K2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="A3:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>